<commit_message>
Added Columns to Asset List
</commit_message>
<xml_diff>
--- a/00_INFOS/ASSET_INFO.xlsx
+++ b/00_INFOS/ASSET_INFO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Oceanpact - Copia\00 - INFOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\EquipmentAnalytics\00_INFOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66468F23-422C-4CF1-B85F-4326A913B349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A39625-2822-4FFD-B43F-CD2FFE8F1530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -100,9 +100,6 @@
     <t>EM1453</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>ABC00575</t>
   </si>
   <si>
@@ -188,6 +185,24 @@
   </si>
   <si>
     <t>Earthshore</t>
+  </si>
+  <si>
+    <t>Contato</t>
+  </si>
+  <si>
+    <t>Analista</t>
+  </si>
+  <si>
+    <t>CSP</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Anna</t>
   </si>
 </sst>
 </file>
@@ -1034,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1065,7 @@
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1075,16 +1090,25 @@
       <c r="H1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1096,21 +1120,30 @@
         <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -1122,21 +1155,30 @@
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -1148,21 +1190,30 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1174,21 +1225,30 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -1200,21 +1260,30 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -1226,21 +1295,30 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1252,21 +1330,30 @@
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -1278,21 +1365,30 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -1304,21 +1400,30 @@
         <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -1330,21 +1435,30 @@
         <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -1356,21 +1470,30 @@
         <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
@@ -1382,21 +1505,30 @@
         <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -1408,21 +1540,30 @@
         <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
@@ -1434,21 +1575,30 @@
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -1460,21 +1610,30 @@
         <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -1486,24 +1645,30 @@
         <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s">
         <v>7</v>
       </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
       <c r="J17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="K17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
@@ -1515,21 +1680,30 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1541,10 +1715,19 @@
         <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H19" t="s">
         <v>7</v>
+      </c>
+      <c r="I19" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Columns to Asset Info
</commit_message>
<xml_diff>
--- a/00_INFOS/ASSET_INFO.xlsx
+++ b/00_INFOS/ASSET_INFO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\EquipmentAnalytics\00_INFOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A39625-2822-4FFD-B43F-CD2FFE8F1530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8BB6DD-C8F9-416B-8DBF-3D2FAD7B4DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>